<commit_message>
Use US data as temporary placeholder for elec/PTCF, indst/PPRiFUfERoIF, and land/AOCoLUPpUA
</commit_message>
<xml_diff>
--- a/InputData/indst/PPRiFUfERoIF/Pot Perc Reduction in Fuel Use from Early Retirement.xlsx
+++ b/InputData/indst/PPRiFUfERoIF/Pot Perc Reduction in Fuel Use from Early Retirement.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\indst\PPRiFUfERoIF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\indst\PPRiFUfERoIF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB605B6-1B8B-45A6-B66A-3BEE01C55C4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="21075" windowHeight="11055"/>
+    <workbookView xWindow="6165" yWindow="-12585" windowWidth="15585" windowHeight="9540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,23 @@
     <sheet name="Results" sheetId="3" r:id="rId3"/>
     <sheet name="PPRiFUfERoIF" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="164">
   <si>
     <t>Industrial Sector Macroeconomic Indicators</t>
   </si>
@@ -511,12 +523,15 @@
   </si>
   <si>
     <t>Perc Fuel Use Reduction (dimensionless)</t>
+  </si>
+  <si>
+    <t>The EU EPS currently uses US EPS values.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -546,7 +561,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -574,6 +589,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -628,7 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -664,6 +685,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -758,6 +781,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -793,6 +833,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -968,10 +1025,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1018,67 +1077,76 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
+      <c r="A10" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="22"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
+      <c r="A11" s="14"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1089,7 +1157,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2758,7 +2826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2888,7 +2956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>

</xml_diff>